<commit_message>
r square & blindfold
</commit_message>
<xml_diff>
--- a/target/smartpls.xlsx
+++ b/target/smartpls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\www\tesis\target\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EA601F-38B3-423E-860B-8EB82090C4D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3D9B8F-EB53-474D-87B8-1111EB2FA7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{A045F930-4DC8-43A3-823B-36ED7A8AB670}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{A045F930-4DC8-43A3-823B-36ED7A8AB670}"/>
   </bookViews>
   <sheets>
     <sheet name="flc" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="validity and reability" sheetId="3" r:id="rId3"/>
     <sheet name="loading factor" sheetId="4" r:id="rId4"/>
     <sheet name="bootstrapping" sheetId="5" r:id="rId5"/>
+    <sheet name="r square" sheetId="6" r:id="rId6"/>
+    <sheet name="blindfold" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="198">
   <si>
     <t>BK (X3)</t>
   </si>
@@ -599,6 +601,30 @@
   </si>
   <si>
     <t>0.397</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>R Square Adjusted</t>
+  </si>
+  <si>
+    <t>0.544</t>
+  </si>
+  <si>
+    <t>0.535</t>
+  </si>
+  <si>
+    <t>SSO</t>
+  </si>
+  <si>
+    <t>SSE</t>
+  </si>
+  <si>
+    <t>Q² (=1-SSE/SSO)</t>
+  </si>
+  <si>
+    <t>0.409</t>
   </si>
 </sst>
 </file>
@@ -1872,7 +1898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D632CE-895E-47EE-8302-B52F9BDA9B35}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G9"/>
     </sheetView>
   </sheetViews>
@@ -2038,4 +2064,155 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4059C2-B032-4359-AABB-26B5B52ACA28}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337DD07D-15D1-4E7C-B810-55956BD8A789}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2250000</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2250000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>375000</v>
+      </c>
+      <c r="C3" s="1">
+        <v>375000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4125000</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4125000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3750000</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3750000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>375000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>375000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3000000</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1772020</v>
+      </c>
+      <c r="D7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2250000</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2250000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>375000</v>
+      </c>
+      <c r="C9" s="1">
+        <v>375000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>